<commit_message>
Added CD/PTUD CSDL 2/ThucHanh/TaiLieu/Tuan#6 - JDBC API - PTUD CSDL 2.docx
</commit_message>
<xml_diff>
--- a/DH/Classes/15HCB/Danh sách đăng kí nhóm 15HCB2 - PTUD HTTT HĐ.xlsx
+++ b/DH/Classes/15HCB/Danh sách đăng kí nhóm 15HCB2 - PTUD HTTT HĐ.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="630" windowWidth="19815" windowHeight="9405"/>
+    <workbookView xWindow="390" yWindow="630" windowWidth="19440" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="DS ĐK Nhóm" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="155">
   <si>
     <t>STT</t>
   </si>
@@ -712,35 +712,10 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -751,8 +726,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1057,8 +1057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40:F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1121,7 +1121,7 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="31" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="5">
@@ -1133,7 +1133,7 @@
       <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="36" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -1144,7 +1144,7 @@
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="22"/>
+      <c r="B3" s="30"/>
       <c r="C3" s="5">
         <v>1542252</v>
       </c>
@@ -1154,7 +1154,7 @@
       <c r="E3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="22"/>
+      <c r="F3" s="30"/>
       <c r="G3" s="3" t="s">
         <v>138</v>
       </c>
@@ -1163,7 +1163,7 @@
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="22"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="5">
         <v>1542253</v>
       </c>
@@ -1173,7 +1173,7 @@
       <c r="E4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="22"/>
+      <c r="F4" s="30"/>
       <c r="G4" s="3" t="s">
         <v>138</v>
       </c>
@@ -1182,7 +1182,7 @@
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="22"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="5">
         <v>1542267</v>
       </c>
@@ -1192,7 +1192,7 @@
       <c r="E5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="22"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="3" t="s">
         <v>138</v>
       </c>
@@ -1201,7 +1201,7 @@
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="22"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="5">
         <v>1542275</v>
       </c>
@@ -1211,7 +1211,7 @@
       <c r="E6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="22"/>
+      <c r="F6" s="30"/>
       <c r="G6" s="3" t="s">
         <v>138</v>
       </c>
@@ -1220,7 +1220,7 @@
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="31" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="5">
@@ -1232,7 +1232,7 @@
       <c r="E7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="36" t="s">
         <v>21</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -1243,7 +1243,7 @@
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="22"/>
+      <c r="B8" s="30"/>
       <c r="C8" s="5">
         <v>1542257</v>
       </c>
@@ -1253,7 +1253,7 @@
       <c r="E8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="22"/>
+      <c r="F8" s="30"/>
       <c r="G8" s="3" t="s">
         <v>139</v>
       </c>
@@ -1262,7 +1262,7 @@
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="22"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="5">
         <v>1542258</v>
       </c>
@@ -1272,7 +1272,7 @@
       <c r="E9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="22"/>
+      <c r="F9" s="30"/>
       <c r="G9" s="3" t="s">
         <v>139</v>
       </c>
@@ -1281,7 +1281,7 @@
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="22"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="5">
         <v>1542251</v>
       </c>
@@ -1291,7 +1291,7 @@
       <c r="E10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="22"/>
+      <c r="F10" s="30"/>
       <c r="G10" s="3" t="s">
         <v>139</v>
       </c>
@@ -1300,7 +1300,7 @@
       <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="22"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="5">
         <v>1542284</v>
       </c>
@@ -1310,7 +1310,7 @@
       <c r="E11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="22"/>
+      <c r="F11" s="30"/>
       <c r="G11" s="3" t="s">
         <v>139</v>
       </c>
@@ -1319,7 +1319,7 @@
       <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="31" t="s">
         <v>30</v>
       </c>
       <c r="C12" s="6">
@@ -1331,7 +1331,7 @@
       <c r="E12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="36" t="s">
         <v>33</v>
       </c>
       <c r="G12" s="20" t="s">
@@ -1342,7 +1342,7 @@
       <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="22"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="6">
         <v>1542241</v>
       </c>
@@ -1352,7 +1352,7 @@
       <c r="E13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="22"/>
+      <c r="F13" s="30"/>
       <c r="G13" s="20" t="s">
         <v>140</v>
       </c>
@@ -1361,7 +1361,7 @@
       <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="22"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="6">
         <v>1542264</v>
       </c>
@@ -1371,7 +1371,7 @@
       <c r="E14" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="22"/>
+      <c r="F14" s="30"/>
       <c r="G14" s="20" t="s">
         <v>140</v>
       </c>
@@ -1380,7 +1380,7 @@
       <c r="A15" s="4">
         <v>16</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="31">
         <v>2017</v>
       </c>
       <c r="C15" s="5">
@@ -1392,7 +1392,7 @@
       <c r="E15" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="36" t="s">
         <v>40</v>
       </c>
       <c r="G15" s="3" t="s">
@@ -1403,7 +1403,7 @@
       <c r="A16" s="4">
         <v>17</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="5">
         <v>1542208</v>
       </c>
@@ -1413,7 +1413,7 @@
       <c r="E16" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="22"/>
+      <c r="F16" s="30"/>
       <c r="G16" s="3" t="s">
         <v>138</v>
       </c>
@@ -1422,7 +1422,7 @@
       <c r="A17" s="4">
         <v>18</v>
       </c>
-      <c r="B17" s="22"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="5">
         <v>1542211</v>
       </c>
@@ -1432,7 +1432,7 @@
       <c r="E17" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F17" s="22"/>
+      <c r="F17" s="30"/>
       <c r="G17" s="3" t="s">
         <v>138</v>
       </c>
@@ -1441,7 +1441,7 @@
       <c r="A18" s="4">
         <v>19</v>
       </c>
-      <c r="B18" s="22"/>
+      <c r="B18" s="30"/>
       <c r="C18" s="5">
         <v>1542268</v>
       </c>
@@ -1451,7 +1451,7 @@
       <c r="E18" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="22"/>
+      <c r="F18" s="30"/>
       <c r="G18" s="3" t="s">
         <v>138</v>
       </c>
@@ -1460,7 +1460,7 @@
       <c r="A19" s="4">
         <v>20</v>
       </c>
-      <c r="B19" s="22"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="5">
         <v>1542285</v>
       </c>
@@ -1470,7 +1470,7 @@
       <c r="E19" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="22"/>
+      <c r="F19" s="30"/>
       <c r="G19" s="3" t="s">
         <v>138</v>
       </c>
@@ -1479,7 +1479,7 @@
       <c r="A20" s="4">
         <v>21</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="31" t="s">
         <v>49</v>
       </c>
       <c r="C20" s="5">
@@ -1491,7 +1491,7 @@
       <c r="E20" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="21" t="s">
+      <c r="F20" s="36" t="s">
         <v>52</v>
       </c>
       <c r="G20" s="3" t="s">
@@ -1502,7 +1502,7 @@
       <c r="A21" s="4">
         <v>22</v>
       </c>
-      <c r="B21" s="22"/>
+      <c r="B21" s="30"/>
       <c r="C21" s="5">
         <v>1542011</v>
       </c>
@@ -1512,7 +1512,7 @@
       <c r="E21" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="22"/>
+      <c r="F21" s="30"/>
       <c r="G21" s="3" t="s">
         <v>139</v>
       </c>
@@ -1521,7 +1521,7 @@
       <c r="A22" s="4">
         <v>23</v>
       </c>
-      <c r="B22" s="22"/>
+      <c r="B22" s="30"/>
       <c r="C22" s="5">
         <v>1542087</v>
       </c>
@@ -1531,7 +1531,7 @@
       <c r="E22" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="22"/>
+      <c r="F22" s="30"/>
       <c r="G22" s="3" t="s">
         <v>139</v>
       </c>
@@ -1540,7 +1540,7 @@
       <c r="A23" s="4">
         <v>24</v>
       </c>
-      <c r="B23" s="22"/>
+      <c r="B23" s="30"/>
       <c r="C23" s="5">
         <v>1542094</v>
       </c>
@@ -1550,7 +1550,7 @@
       <c r="E23" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="22"/>
+      <c r="F23" s="30"/>
       <c r="G23" s="3" t="s">
         <v>139</v>
       </c>
@@ -1559,7 +1559,7 @@
       <c r="A24" s="4">
         <v>25</v>
       </c>
-      <c r="B24" s="22"/>
+      <c r="B24" s="30"/>
       <c r="C24" s="5">
         <v>1542104</v>
       </c>
@@ -1569,7 +1569,7 @@
       <c r="E24" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F24" s="22"/>
+      <c r="F24" s="30"/>
       <c r="G24" s="3" t="s">
         <v>139</v>
       </c>
@@ -1578,7 +1578,7 @@
       <c r="A25" s="4">
         <v>26</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="31" t="s">
         <v>61</v>
       </c>
       <c r="C25" s="9">
@@ -1590,7 +1590,7 @@
       <c r="E25" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F25" s="21" t="s">
+      <c r="F25" s="36" t="s">
         <v>64</v>
       </c>
       <c r="G25" s="20" t="s">
@@ -1601,7 +1601,7 @@
       <c r="A26" s="4">
         <v>27</v>
       </c>
-      <c r="B26" s="22"/>
+      <c r="B26" s="30"/>
       <c r="C26" s="9">
         <v>1542255</v>
       </c>
@@ -1611,7 +1611,7 @@
       <c r="E26" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="F26" s="22"/>
+      <c r="F26" s="30"/>
       <c r="G26" s="20" t="s">
         <v>140</v>
       </c>
@@ -1620,7 +1620,7 @@
       <c r="A27" s="4">
         <v>28</v>
       </c>
-      <c r="B27" s="22"/>
+      <c r="B27" s="30"/>
       <c r="C27" s="9">
         <v>1542205</v>
       </c>
@@ -1630,7 +1630,7 @@
       <c r="E27" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="F27" s="22"/>
+      <c r="F27" s="30"/>
       <c r="G27" s="20" t="s">
         <v>140</v>
       </c>
@@ -1639,7 +1639,7 @@
       <c r="A28" s="4">
         <v>29</v>
       </c>
-      <c r="B28" s="22"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="9">
         <v>1542227</v>
       </c>
@@ -1649,7 +1649,7 @@
       <c r="E28" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F28" s="22"/>
+      <c r="F28" s="30"/>
       <c r="G28" s="20" t="s">
         <v>140</v>
       </c>
@@ -1658,7 +1658,7 @@
       <c r="A29" s="4">
         <v>30</v>
       </c>
-      <c r="B29" s="22"/>
+      <c r="B29" s="30"/>
       <c r="C29" s="5">
         <v>1542287</v>
       </c>
@@ -1668,7 +1668,7 @@
       <c r="E29" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F29" s="22"/>
+      <c r="F29" s="30"/>
       <c r="G29" s="20" t="s">
         <v>140</v>
       </c>
@@ -1677,7 +1677,7 @@
       <c r="A30" s="4">
         <v>31</v>
       </c>
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="31" t="s">
         <v>73</v>
       </c>
       <c r="C30" s="5">
@@ -1689,7 +1689,7 @@
       <c r="E30" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F30" s="21" t="s">
+      <c r="F30" s="36" t="s">
         <v>76</v>
       </c>
       <c r="G30" s="3" t="s">
@@ -1700,7 +1700,7 @@
       <c r="A31" s="4">
         <v>32</v>
       </c>
-      <c r="B31" s="22"/>
+      <c r="B31" s="30"/>
       <c r="C31" s="5">
         <v>1542223</v>
       </c>
@@ -1710,7 +1710,7 @@
       <c r="E31" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="F31" s="22"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="3" t="s">
         <v>138</v>
       </c>
@@ -1719,7 +1719,7 @@
       <c r="A32" s="4">
         <v>33</v>
       </c>
-      <c r="B32" s="22"/>
+      <c r="B32" s="30"/>
       <c r="C32" s="5">
         <v>1542282</v>
       </c>
@@ -1729,7 +1729,7 @@
       <c r="E32" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F32" s="22"/>
+      <c r="F32" s="30"/>
       <c r="G32" s="3" t="s">
         <v>138</v>
       </c>
@@ -1738,7 +1738,7 @@
       <c r="A33" s="4">
         <v>34</v>
       </c>
-      <c r="B33" s="22"/>
+      <c r="B33" s="30"/>
       <c r="C33" s="5">
         <v>1542226</v>
       </c>
@@ -1748,7 +1748,7 @@
       <c r="E33" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="F33" s="22"/>
+      <c r="F33" s="30"/>
       <c r="G33" s="3" t="s">
         <v>138</v>
       </c>
@@ -1757,7 +1757,7 @@
       <c r="A34" s="4">
         <v>35</v>
       </c>
-      <c r="B34" s="22"/>
+      <c r="B34" s="30"/>
       <c r="C34" s="5">
         <v>1542289</v>
       </c>
@@ -1767,7 +1767,7 @@
       <c r="E34" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="F34" s="22"/>
+      <c r="F34" s="30"/>
       <c r="G34" s="3" t="s">
         <v>138</v>
       </c>
@@ -1776,7 +1776,7 @@
       <c r="A35" s="4">
         <v>36</v>
       </c>
-      <c r="B35" s="24" t="s">
+      <c r="B35" s="31" t="s">
         <v>85</v>
       </c>
       <c r="C35" s="12">
@@ -1788,7 +1788,7 @@
       <c r="E35" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F35" s="21" t="s">
+      <c r="F35" s="36" t="s">
         <v>88</v>
       </c>
       <c r="G35" s="3" t="s">
@@ -1799,7 +1799,7 @@
       <c r="A36" s="4">
         <v>37</v>
       </c>
-      <c r="B36" s="22"/>
+      <c r="B36" s="30"/>
       <c r="C36" s="12">
         <v>1542019</v>
       </c>
@@ -1809,7 +1809,7 @@
       <c r="E36" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="F36" s="22"/>
+      <c r="F36" s="30"/>
       <c r="G36" s="3" t="s">
         <v>139</v>
       </c>
@@ -1818,7 +1818,7 @@
       <c r="A37" s="4">
         <v>38</v>
       </c>
-      <c r="B37" s="22"/>
+      <c r="B37" s="30"/>
       <c r="C37" s="12">
         <v>1542075</v>
       </c>
@@ -1828,7 +1828,7 @@
       <c r="E37" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F37" s="22"/>
+      <c r="F37" s="30"/>
       <c r="G37" s="3" t="s">
         <v>139</v>
       </c>
@@ -1837,7 +1837,7 @@
       <c r="A38" s="4">
         <v>39</v>
       </c>
-      <c r="B38" s="22"/>
+      <c r="B38" s="30"/>
       <c r="C38" s="12">
         <v>1542088</v>
       </c>
@@ -1847,7 +1847,7 @@
       <c r="E38" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="F38" s="22"/>
+      <c r="F38" s="30"/>
       <c r="G38" s="3" t="s">
         <v>139</v>
       </c>
@@ -1856,7 +1856,7 @@
       <c r="A39" s="4">
         <v>40</v>
       </c>
-      <c r="B39" s="22"/>
+      <c r="B39" s="30"/>
       <c r="C39" s="12">
         <v>1542021</v>
       </c>
@@ -1866,7 +1866,7 @@
       <c r="E39" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="F39" s="22"/>
+      <c r="F39" s="30"/>
       <c r="G39" s="3" t="s">
         <v>139</v>
       </c>
@@ -1875,7 +1875,7 @@
       <c r="A40" s="4">
         <v>41</v>
       </c>
-      <c r="B40" s="24" t="s">
+      <c r="B40" s="31" t="s">
         <v>97</v>
       </c>
       <c r="C40" s="12">
@@ -1887,7 +1887,7 @@
       <c r="E40" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="F40" s="23" t="s">
+      <c r="F40" s="29" t="s">
         <v>100</v>
       </c>
       <c r="G40" s="20" t="s">
@@ -1898,7 +1898,7 @@
       <c r="A41" s="4">
         <v>42</v>
       </c>
-      <c r="B41" s="22"/>
+      <c r="B41" s="30"/>
       <c r="C41" s="12">
         <v>1542232</v>
       </c>
@@ -1908,7 +1908,7 @@
       <c r="E41" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="F41" s="22"/>
+      <c r="F41" s="30"/>
       <c r="G41" s="20" t="s">
         <v>140</v>
       </c>
@@ -1917,7 +1917,7 @@
       <c r="A42" s="4">
         <v>43</v>
       </c>
-      <c r="B42" s="22"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="12">
         <v>1542266</v>
       </c>
@@ -1927,7 +1927,7 @@
       <c r="E42" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="F42" s="22"/>
+      <c r="F42" s="30"/>
       <c r="G42" s="20" t="s">
         <v>140</v>
       </c>
@@ -1936,7 +1936,7 @@
       <c r="A43" s="4">
         <v>44</v>
       </c>
-      <c r="B43" s="22"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="12">
         <v>1542248</v>
       </c>
@@ -1946,7 +1946,7 @@
       <c r="E43" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="F43" s="22"/>
+      <c r="F43" s="30"/>
       <c r="G43" s="20" t="s">
         <v>140</v>
       </c>
@@ -1955,7 +1955,7 @@
       <c r="A44" s="4">
         <v>45</v>
       </c>
-      <c r="B44" s="22"/>
+      <c r="B44" s="30"/>
       <c r="C44" s="12">
         <v>1542293</v>
       </c>
@@ -1965,7 +1965,7 @@
       <c r="E44" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="F44" s="22"/>
+      <c r="F44" s="30"/>
       <c r="G44" s="20" t="s">
         <v>140</v>
       </c>
@@ -1974,7 +1974,7 @@
       <c r="A45" s="14">
         <v>46</v>
       </c>
-      <c r="B45" s="24" t="s">
+      <c r="B45" s="31" t="s">
         <v>109</v>
       </c>
       <c r="C45" s="15">
@@ -1986,7 +1986,7 @@
       <c r="E45" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="F45" s="23" t="s">
+      <c r="F45" s="29" t="s">
         <v>112</v>
       </c>
       <c r="G45" s="3" t="s">
@@ -1997,7 +1997,7 @@
       <c r="A46" s="14">
         <v>47</v>
       </c>
-      <c r="B46" s="22"/>
+      <c r="B46" s="30"/>
       <c r="C46" s="15">
         <v>1542245</v>
       </c>
@@ -2007,7 +2007,7 @@
       <c r="E46" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="F46" s="22"/>
+      <c r="F46" s="30"/>
       <c r="G46" s="3" t="s">
         <v>138</v>
       </c>
@@ -2016,7 +2016,7 @@
       <c r="A47" s="14">
         <v>48</v>
       </c>
-      <c r="B47" s="22"/>
+      <c r="B47" s="30"/>
       <c r="C47" s="15">
         <v>1542247</v>
       </c>
@@ -2026,7 +2026,7 @@
       <c r="E47" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="F47" s="22"/>
+      <c r="F47" s="30"/>
       <c r="G47" s="3" t="s">
         <v>138</v>
       </c>
@@ -2035,7 +2035,7 @@
       <c r="A48" s="14">
         <v>49</v>
       </c>
-      <c r="B48" s="22"/>
+      <c r="B48" s="30"/>
       <c r="C48" s="15">
         <v>1542277</v>
       </c>
@@ -2045,7 +2045,7 @@
       <c r="E48" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="F48" s="22"/>
+      <c r="F48" s="30"/>
       <c r="G48" s="3" t="s">
         <v>138</v>
       </c>
@@ -2054,15 +2054,15 @@
       <c r="A49" s="14">
         <v>50</v>
       </c>
-      <c r="B49" s="22"/>
+      <c r="B49" s="30"/>
       <c r="C49" s="16">
         <v>1542234</v>
       </c>
-      <c r="D49" s="29" t="s">
+      <c r="D49" s="22" t="s">
         <v>143</v>
       </c>
       <c r="E49" s="16"/>
-      <c r="F49" s="22"/>
+      <c r="F49" s="30"/>
       <c r="G49" s="3" t="s">
         <v>138</v>
       </c>
@@ -2071,7 +2071,7 @@
       <c r="A50" s="18">
         <v>51</v>
       </c>
-      <c r="B50" s="24" t="s">
+      <c r="B50" s="31" t="s">
         <v>119</v>
       </c>
       <c r="C50" s="16">
@@ -2083,7 +2083,7 @@
       <c r="E50" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="F50" s="23" t="s">
+      <c r="F50" s="29" t="s">
         <v>122</v>
       </c>
       <c r="G50" s="3" t="s">
@@ -2094,7 +2094,7 @@
       <c r="A51" s="14">
         <v>52</v>
       </c>
-      <c r="B51" s="22"/>
+      <c r="B51" s="30"/>
       <c r="C51" s="16">
         <v>1542239</v>
       </c>
@@ -2104,7 +2104,7 @@
       <c r="E51" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="F51" s="22"/>
+      <c r="F51" s="30"/>
       <c r="G51" s="3" t="s">
         <v>139</v>
       </c>
@@ -2113,7 +2113,7 @@
       <c r="A52" s="19">
         <v>53</v>
       </c>
-      <c r="B52" s="22"/>
+      <c r="B52" s="30"/>
       <c r="C52" s="15">
         <v>1542291</v>
       </c>
@@ -2123,7 +2123,7 @@
       <c r="E52" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="F52" s="22"/>
+      <c r="F52" s="30"/>
       <c r="G52" s="3" t="s">
         <v>139</v>
       </c>
@@ -2132,7 +2132,7 @@
       <c r="A53" s="19">
         <v>54</v>
       </c>
-      <c r="B53" s="22"/>
+      <c r="B53" s="30"/>
       <c r="C53" s="15">
         <v>1542022</v>
       </c>
@@ -2142,7 +2142,7 @@
       <c r="E53" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="F53" s="22"/>
+      <c r="F53" s="30"/>
       <c r="G53" s="3" t="s">
         <v>139</v>
       </c>
@@ -2151,7 +2151,7 @@
       <c r="A54" s="14">
         <v>55</v>
       </c>
-      <c r="B54" s="30" t="s">
+      <c r="B54" s="27" t="s">
         <v>129</v>
       </c>
       <c r="C54" s="15">
@@ -2163,7 +2163,7 @@
       <c r="E54" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="F54" s="26" t="s">
+      <c r="F54" s="32" t="s">
         <v>132</v>
       </c>
       <c r="G54" s="20" t="s">
@@ -2174,7 +2174,7 @@
       <c r="A55" s="14">
         <v>56</v>
       </c>
-      <c r="B55" s="31"/>
+      <c r="B55" s="28"/>
       <c r="C55" s="15">
         <v>1542249</v>
       </c>
@@ -2184,7 +2184,7 @@
       <c r="E55" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="F55" s="27"/>
+      <c r="F55" s="33"/>
       <c r="G55" s="20" t="s">
         <v>140</v>
       </c>
@@ -2193,7 +2193,7 @@
       <c r="A56" s="14">
         <v>57</v>
       </c>
-      <c r="B56" s="31"/>
+      <c r="B56" s="28"/>
       <c r="C56" s="15">
         <v>1442084</v>
       </c>
@@ -2203,7 +2203,7 @@
       <c r="E56" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="F56" s="27"/>
+      <c r="F56" s="33"/>
       <c r="G56" s="20" t="s">
         <v>140</v>
       </c>
@@ -2212,17 +2212,17 @@
       <c r="A57" s="14">
         <v>58</v>
       </c>
-      <c r="B57" s="32"/>
+      <c r="B57" s="35"/>
       <c r="C57" s="15">
         <v>1542271</v>
       </c>
-      <c r="D57" s="25" t="s">
+      <c r="D57" s="21" t="s">
         <v>141</v>
       </c>
       <c r="E57" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="F57" s="28"/>
+      <c r="F57" s="34"/>
       <c r="G57" s="20" t="s">
         <v>140</v>
       </c>
@@ -2231,53 +2231,62 @@
       <c r="A58" s="14">
         <v>59</v>
       </c>
-      <c r="B58" s="30" t="s">
+      <c r="B58" s="27" t="s">
         <v>154</v>
       </c>
       <c r="C58" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="D58" s="36" t="s">
+      <c r="D58" s="23" t="s">
         <v>145</v>
       </c>
       <c r="E58" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="F58" s="33" t="s">
+      <c r="F58" s="24" t="s">
         <v>153</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="14">
         <v>60</v>
       </c>
-      <c r="B59" s="31"/>
+      <c r="B59" s="28"/>
       <c r="C59" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="D59" s="36" t="s">
+      <c r="D59" s="23" t="s">
         <v>147</v>
       </c>
       <c r="E59" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="F59" s="34"/>
+      <c r="F59" s="25"/>
+      <c r="G59" s="3" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="60" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="14">
         <v>61</v>
       </c>
-      <c r="B60" s="31"/>
+      <c r="B60" s="28"/>
       <c r="C60" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="D60" s="36" t="s">
+      <c r="D60" s="23" t="s">
         <v>148</v>
       </c>
       <c r="E60" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="F60" s="35"/>
+      <c r="F60" s="26"/>
+      <c r="G60" s="3" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="61" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="14"/>
@@ -9793,6 +9802,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="F15:F19"/>
+    <mergeCell ref="F20:F24"/>
+    <mergeCell ref="F2:F6"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="F45:F49"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="F35:F39"/>
+    <mergeCell ref="F40:F44"/>
+    <mergeCell ref="F25:F29"/>
+    <mergeCell ref="F30:F34"/>
     <mergeCell ref="F58:F60"/>
     <mergeCell ref="B58:B60"/>
     <mergeCell ref="F50:F53"/>
@@ -9809,16 +9828,6 @@
     <mergeCell ref="B50:B53"/>
     <mergeCell ref="F54:F57"/>
     <mergeCell ref="B54:B57"/>
-    <mergeCell ref="F15:F19"/>
-    <mergeCell ref="F20:F24"/>
-    <mergeCell ref="F2:F6"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="F45:F49"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="F35:F39"/>
-    <mergeCell ref="F40:F44"/>
-    <mergeCell ref="F25:F29"/>
-    <mergeCell ref="F30:F34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>

</xml_diff>